<commit_message>
Update paper output to include revised plots
</commit_message>
<xml_diff>
--- a/paper_output/CaseI/CaseI_main/CaseI_parameter_table.xlsx
+++ b/paper_output/CaseI/CaseI_main/CaseI_parameter_table.xlsx
@@ -507,7 +507,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.4E-04\(\pm\)6E-07</t>
+          <t>2.4E-04\(\pm\)7E-07</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -517,12 +517,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.9E-04\(\pm\)3E-07</t>
+          <t>1.9E-04\(\pm\)4E-07</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4.7E-05\(\pm\)4E-08</t>
+          <t>4.7E-05\(\pm\)8E-08</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9.1E-02\(\pm\)3E-05</t>
+          <t>9.1E-02\(\pm\)5E-05</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>9.3E-02\(\pm\)7E-05</t>
+          <t>9.3E-02\(\pm\)8E-05</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -568,27 +568,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3.0E-05\(\pm\)3E-08</t>
+          <t>3.0E-05\(\pm\)2E-08</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.9E-05\(\pm\)4E-08</t>
+          <t>1.9E-05\(\pm\)3E-08</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1.2E-05\(\pm\)3E-08</t>
+          <t>1.2E-05\(\pm\)4E-08</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1.7E-05\(\pm\)5E-08</t>
+          <t>1.7E-05\(\pm\)4E-08</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>9.3E-06\(\pm\)3E-08</t>
+          <t>9.3E-06\(\pm\)2E-08</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4.8E-02\(\pm\)8E-06</t>
+          <t>4.8E-02\(\pm\)6E-06</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)2E-05</t>
+          <t>5.5E-02\(\pm\)3E-05</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>5.8E-02\(\pm\)3E-05</t>
+          <t>5.8E-02\(\pm\)2E-05</t>
         </is>
       </c>
     </row>
@@ -639,17 +639,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)8E-05</t>
+          <t>5.5E-02\(\pm\)6E-05</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>5.0E-02\(\pm\)2E-05</t>
+          <t>5.0E-02\(\pm\)5E-05</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>7.9E-02\(\pm\)2E-04</t>
+          <t>7.9E-02\(\pm\)3E-04</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -667,22 +667,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1.5E-02\(\pm\)1E-05</t>
+          <t>1.5E-02\(\pm\)2E-05</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.0E-02\(\pm\)3E-05</t>
+          <t>1.0E-02\(\pm\)4E-05</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.0E-02\(\pm\)1E-05</t>
+          <t>1.0E-02\(\pm\)2E-05</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1.7E-02\(\pm\)7E-05</t>
+          <t>1.8E-02\(\pm\)5E-05</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>3.6E-02\(\pm\)7E-05</t>
+          <t>3.6E-02\(\pm\)4E-05</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -759,7 +759,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>0.502920881579502</v>
+        <v>0.5</v>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
@@ -768,27 +768,27 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2.2E-04\(\pm\)1E-07</t>
+          <t>2.2E-04\(\pm\)2E-07</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.5E-04\(\pm\)4E-07</t>
+          <t>2.5E-04\(\pm\)6E-07</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2.0E-04\(\pm\)5E-07</t>
+          <t>2.0E-04\(\pm\)6E-07</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2.1E-04\(\pm\)3E-07</t>
+          <t>2.1E-04\(\pm\)4E-07</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>6.9E-05\(\pm\)1E-07</t>
+          <t>6.9E-05\(\pm\)2E-07</t>
         </is>
       </c>
     </row>
@@ -806,22 +806,22 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>8.5E-02\(\pm\)6E-05</t>
+          <t>8.5E-02\(\pm\)8E-05</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>7.9E-02\(\pm\)4E-05</t>
+          <t>8.0E-02\(\pm\)6E-05</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>8.7E-02\(\pm\)7E-05</t>
+          <t>8.8E-02\(\pm\)7E-05</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>9.7E-02\(\pm\)4E-05</t>
+          <t>9.7E-02\(\pm\)6E-05</t>
         </is>
       </c>
     </row>
@@ -834,22 +834,22 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3.7E-05\(\pm\)3E-08</t>
+          <t>3.7E-05\(\pm\)2E-08</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3.4E-05\(\pm\)6E-08</t>
+          <t>3.4E-05\(\pm\)5E-08</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3.6E-05\(\pm\)4E-08</t>
+          <t>3.6E-05\(\pm\)6E-08</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>3.6E-05\(\pm\)7E-08</t>
+          <t>3.6E-05\(\pm\)6E-08</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5.0E-02\(\pm\)8E-06</t>
+          <t>5.0E-02\(\pm\)4E-06</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -877,17 +877,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5.0E-02\(\pm\)1E-05</t>
+          <t>5.0E-02\(\pm\)2E-05</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>5.1E-02\(\pm\)2E-05</t>
+          <t>5.1E-02\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>5.3E-02\(\pm\)1E-05</t>
+          <t>5.3E-02\(\pm\)9E-06</t>
         </is>
       </c>
     </row>
@@ -900,17 +900,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7.6E-02\(\pm\)5E-05</t>
+          <t>7.5E-02\(\pm\)7E-05</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>7.6E-02\(\pm\)1E-04</t>
+          <t>7.5E-02\(\pm\)6E-05</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6.8E-02\(\pm\)3E-05</t>
+          <t>6.8E-02\(\pm\)6E-05</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -938,17 +938,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>9.0E-03\(\pm\)2E-05</t>
+          <t>9.0E-03\(\pm\)3E-05</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>9.7E-03\(\pm\)6E-06</t>
+          <t>9.7E-03\(\pm\)2E-05</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>1.1E-02\(\pm\)4E-05</t>
+          <t>1.1E-02\(\pm\)3E-05</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -966,22 +966,22 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>9.3E-03\(\pm\)6E-06</t>
+          <t>9.3E-03\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>8.2E-03\(\pm\)1E-05</t>
+          <t>8.2E-03\(\pm\)7E-06</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>6.8E-03\(\pm\)6E-06</t>
+          <t>6.8E-03\(\pm\)8E-06</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>1.0E-02\(\pm\)2E-05</t>
+          <t>1.0E-02\(\pm\)3E-05</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1009,17 +1009,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4.0E-02\(\pm\)2E-05</t>
+          <t>4.0E-02\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>3.5E-02\(\pm\)4E-05</t>
+          <t>3.5E-02\(\pm\)3E-05</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>3.8E-02\(\pm\)1E-05</t>
+          <t>3.8E-02\(\pm\)2E-05</t>
         </is>
       </c>
     </row>
@@ -1034,27 +1034,27 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2.3E-04\(\pm\)1E-07</t>
+          <t>2.3E-04\(\pm\)2E-07</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>2.3E-04\(\pm\)4E-07</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2.3E-04\(\pm\)6E-07</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>2.3E-04\(\pm\)3E-07</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2.3E-04\(\pm\)3E-07</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2.3E-04\(\pm\)2E-07</t>
-        </is>
-      </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2.3E-04\(\pm\)5E-07</t>
+          <t>2.3E-04\(\pm\)6E-07</t>
         </is>
       </c>
     </row>
@@ -1072,22 +1072,22 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>7.0E-02\(\pm\)7E-05</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>7.0E-02\(\pm\)5E-05</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>7.0E-02\(\pm\)5E-05</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>7.0E-02\(\pm\)6E-05</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>7.0E-02\(\pm\)3E-05</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>7.0E-02\(\pm\)7E-05</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>7.0E-02\(\pm\)5E-05</t>
         </is>
       </c>
     </row>
@@ -1100,27 +1100,27 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3.4E-05\(\pm\)3E-08</t>
+          <t>3.4E-05\(\pm\)1E-08</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3.4E-05\(\pm\)7E-08</t>
+          <t>3.4E-05\(\pm\)4E-08</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3.4E-05\(\pm\)3E-08</t>
+          <t>3.4E-05\(\pm\)5E-08</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>3.4E-05\(\pm\)8E-08</t>
+          <t>3.4E-05\(\pm\)5E-08</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>3.4E-05\(\pm\)4E-08</t>
+          <t>3.4E-05\(\pm\)2E-08</t>
         </is>
       </c>
     </row>
@@ -1133,27 +1133,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)9E-06</t>
+          <t>5.5E-02\(\pm\)5E-06</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)2E-05</t>
+          <t>5.5E-02\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)8E-06</t>
+          <t>5.5E-02\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)2E-05</t>
+          <t>5.5E-02\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)1E-05</t>
+          <t>5.5E-02\(\pm\)5E-06</t>
         </is>
       </c>
     </row>
@@ -1166,27 +1166,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>8.7E-02\(\pm\)7E-05</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>8.7E-02\(\pm\)8E-05</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>8.7E-02\(\pm\)6E-05</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>8.7E-02\(\pm\)1E-04</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>8.7E-02\(\pm\)4E-05</t>
-        </is>
-      </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>8.7E-02\(\pm\)2E-04</t>
+          <t>8.7E-02\(\pm\)3E-04</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>8.7E-02\(\pm\)7E-05</t>
+          <t>8.7E-02\(\pm\)6E-05</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>8.9E-03\(\pm\)5E-06</t>
+          <t>8.9E-03\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>8.9E-03\(\pm\)8E-06</t>
+          <t>8.9E-03\(\pm\)1E-05</t>
         </is>
       </c>
     </row>
@@ -1232,27 +1232,27 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>5.1E-03\(\pm\)3E-06</t>
+          <t>5.2E-03\(\pm\)6E-06</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5.2E-03\(\pm\)5E-06</t>
+          <t>5.2E-03\(\pm\)4E-06</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5.1E-03\(\pm\)3E-06</t>
+          <t>5.2E-03\(\pm\)4E-06</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>5.2E-03\(\pm\)1E-05</t>
+          <t>5.1E-03\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>5.2E-03\(\pm\)7E-06</t>
+          <t>5.2E-03\(\pm\)4E-06</t>
         </is>
       </c>
     </row>
@@ -1265,19 +1265,19 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>3.2E-02\(\pm\)9E-06</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>3.2E-02\(\pm\)2E-05</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>3.2E-02\(\pm\)8E-06</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>3.2E-02\(\pm\)9E-06</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>3.2E-02\(\pm\)9E-06</t>
-        </is>
-      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>3.2E-02\(\pm\)3E-05</t>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>3.2E-02\(\pm\)9E-06</t>
+          <t>3.2E-02\(\pm\)1E-05</t>
         </is>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2.3E-04\(\pm\)1E-07</t>
+          <t>2.3E-04\(\pm\)2E-07</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1310,17 +1310,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2.3E-04\(\pm\)3E-07</t>
+          <t>2.3E-04\(\pm\)7E-07</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2.1E-04\(\pm\)2E-07</t>
+          <t>2.1E-04\(\pm\)3E-07</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>3.4E-04\(\pm\)5E-07</t>
+          <t>3.4E-04\(\pm\)6E-07</t>
         </is>
       </c>
     </row>
@@ -1333,27 +1333,27 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>6.8E-02\(\pm\)2E-05</t>
+          <t>6.8E-02\(\pm\)3E-05</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6.0E-02\(\pm\)5E-05</t>
+          <t>6.1E-02\(\pm\)7E-05</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>7.0E-02\(\pm\)3E-05</t>
+          <t>7.0E-02\(\pm\)6E-05</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>5.8E-02\(\pm\)6E-05</t>
+          <t>5.8E-02\(\pm\)5E-05</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>6.0E-02\(\pm\)3E-05</t>
+          <t>6.0E-02\(\pm\)4E-05</t>
         </is>
       </c>
     </row>
@@ -1366,27 +1366,27 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>3.0E-05\(\pm\)3E-08</t>
+          <t>3.0E-05\(\pm\)1E-08</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3.0E-05\(\pm\)7E-08</t>
+          <t>3.0E-05\(\pm\)4E-08</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2.5E-05\(\pm\)2E-08</t>
+          <t>2.5E-05\(\pm\)4E-08</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2.8E-05\(\pm\)7E-08</t>
+          <t>2.8E-05\(\pm\)5E-08</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>3.4E-05\(\pm\)4E-08</t>
+          <t>3.4E-05\(\pm\)2E-08</t>
         </is>
       </c>
     </row>
@@ -1399,27 +1399,27 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>5.9E-02\(\pm\)9E-06</t>
+          <t>5.9E-02\(\pm\)5E-06</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>5.8E-02\(\pm\)1E-05</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>6.0E-02\(\pm\)1E-05</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
           <t>5.8E-02\(\pm\)2E-05</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>6.0E-02\(\pm\)7E-06</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>5.8E-02\(\pm\)2E-05</t>
-        </is>
-      </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>5.8E-02\(\pm\)1E-05</t>
+          <t>5.8E-02\(\pm\)6E-06</t>
         </is>
       </c>
     </row>
@@ -1432,27 +1432,27 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>9.0E-02\(\pm\)7E-05</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>8.9E-02\(\pm\)8E-05</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>9.5E-02\(\pm\)7E-05</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>9.5E-02\(\pm\)3E-04</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>9.0E-02\(\pm\)5E-05</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>8.9E-02\(\pm\)1E-04</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>9.5E-02\(\pm\)4E-05</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>9.5E-02\(\pm\)2E-04</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>9.0E-02\(\pm\)7E-05</t>
         </is>
       </c>
     </row>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1.0E-02\(\pm\)9E-06</t>
+          <t>1.0E-02\(\pm\)6E-06</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1475,12 +1475,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>9.0E-03\(\pm\)6E-06</t>
+          <t>9.0E-03\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>8.6E-03\(\pm\)3E-05</t>
+          <t>8.6E-03\(\pm\)4E-05</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1498,12 +1498,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2.6E-03\(\pm\)2E-06</t>
+          <t>2.6E-03\(\pm\)3E-06</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.9E-03\(\pm\)3E-06</t>
+          <t>2.9E-03\(\pm\)2E-06</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1513,12 +1513,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2.8E-03\(\pm\)7E-06</t>
+          <t>2.8E-03\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2.7E-03\(\pm\)3E-06</t>
+          <t>2.7E-03\(\pm\)2E-06</t>
         </is>
       </c>
     </row>
@@ -1531,12 +1531,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2.7E-02\(\pm\)6E-06</t>
+          <t>2.7E-02\(\pm\)8E-06</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2.7E-02\(\pm\)1E-05</t>
+          <t>2.7E-02\(\pm\)2E-05</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1566,7 +1566,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2.3E-04\(\pm\)1E-07</t>
+          <t>2.3E-04\(\pm\)2E-07</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2.3E-04\(\pm\)3E-07</t>
+          <t>2.3E-04\(\pm\)8E-07</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1599,22 +1599,22 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>6.6E-02\(\pm\)2E-05</t>
+          <t>6.6E-02\(\pm\)3E-05</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>5.7E-02\(\pm\)5E-05</t>
+          <t>5.7E-02\(\pm\)6E-05</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>7.0E-02\(\pm\)3E-05</t>
+          <t>7.0E-02\(\pm\)6E-05</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>5.5E-02\(\pm\)5E-05</t>
+          <t>5.5E-02\(\pm\)4E-05</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1632,27 +1632,27 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2.9E-05\(\pm\)3E-08</t>
+          <t>2.9E-05\(\pm\)1E-08</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2.8E-05\(\pm\)7E-08</t>
+          <t>2.8E-05\(\pm\)4E-08</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2.3E-05\(\pm\)2E-08</t>
+          <t>2.3E-05\(\pm\)4E-08</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2.6E-05\(\pm\)6E-08</t>
+          <t>2.6E-05\(\pm\)5E-08</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>3.3E-05\(\pm\)4E-08</t>
+          <t>3.3E-05\(\pm\)2E-08</t>
         </is>
       </c>
     </row>
@@ -1665,27 +1665,27 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>6.1E-02\(\pm\)9E-06</t>
+          <t>6.1E-02\(\pm\)5E-06</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
+          <t>6.0E-02\(\pm\)1E-05</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>6.2E-02\(\pm\)1E-05</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
           <t>6.0E-02\(\pm\)2E-05</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>6.2E-02\(\pm\)8E-06</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>6.0E-02\(\pm\)2E-05</t>
-        </is>
-      </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>5.9E-02\(\pm\)1E-05</t>
+          <t>5.9E-02\(\pm\)6E-06</t>
         </is>
       </c>
     </row>
@@ -1698,27 +1698,27 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>9.4E-02\(\pm\)5E-05</t>
+          <t>9.4E-02\(\pm\)7E-05</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>9.1E-02\(\pm\)1E-04</t>
+          <t>9.1E-02\(\pm\)9E-05</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>9.7E-02\(\pm\)4E-05</t>
+          <t>9.7E-02\(\pm\)7E-05</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>9.9E-02\(\pm\)2E-04</t>
+          <t>9.9E-02\(\pm\)4E-04</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>9.6E-02\(\pm\)6E-05</t>
+          <t>9.6E-02\(\pm\)5E-05</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1.1E-02\(\pm\)8E-06</t>
+          <t>1.1E-02\(\pm\)5E-06</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>9.1E-03\(\pm\)6E-06</t>
+          <t>9.1E-03\(\pm\)1E-05</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>1.0E-02\(\pm\)7E-06</t>
+          <t>1.0E-02\(\pm\)6E-06</t>
         </is>
       </c>
     </row>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1.4E-03\(\pm\)7E-07</t>
+          <t>1.4E-03\(\pm\)1E-06</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1774,12 +1774,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1.5E-03\(\pm\)8E-07</t>
+          <t>1.5E-03\(\pm\)1E-06</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>1.5E-03\(\pm\)4E-06</t>
+          <t>1.5E-03\(\pm\)5E-06</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2.5E-02\(\pm\)6E-06</t>
+          <t>2.5E-02\(\pm\)8E-06</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2.5E-02\(\pm\)8E-06</t>
+          <t>2.5E-02\(\pm\)7E-06</t>
         </is>
       </c>
     </row>

</xml_diff>